<commit_message>
trying change happy config
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/HAPPY.xlsx
+++ b/invoice_gen/TEMPLATE/HAPPY.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\gen_inv\TEMPLATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\automate invoice\invoice_gen\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37190551-B9A0-4219-8F23-91FC2C4DD644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E34C8C-8771-4515-B5E2-4BAC69FF3155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="10" r:id="rId1"/>
@@ -22,7 +22,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$1:$F$34</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$G$31</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$G$29</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Packing list'!$A$1:$I$29</definedName>
   </definedNames>
   <calcPr calcId="191029" fullPrecision="0"/>
@@ -598,7 +598,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -750,12 +750,6 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -765,6 +759,12 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -774,11 +774,20 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -788,33 +797,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -828,6 +810,18 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -855,13 +849,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>203200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>179236</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>347731</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -877,7 +871,7 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10679029" y="10961437"/>
+          <a:off x="10679029" y="10008937"/>
           <a:ext cx="3025707" cy="1327636"/>
           <a:chOff x="7095490" y="13465334"/>
           <a:chExt cx="4610436" cy="2150203"/>
@@ -1366,13 +1360,13 @@
       <c r="A12" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="63" t="s">
+      <c r="B12" s="58" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
+      <c r="C12" s="58"/>
+      <c r="D12" s="58"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="58"/>
     </row>
     <row r="13" spans="1:6" s="37" customFormat="1" ht="30" customHeight="1">
       <c r="A13" s="34" t="s">
@@ -1423,24 +1417,24 @@
       <c r="F16" s="33"/>
     </row>
     <row r="17" spans="1:6" s="31" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A17" s="59" t="s">
+      <c r="A17" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="59"/>
-      <c r="C17" s="59"/>
-      <c r="D17" s="59"/>
-      <c r="E17" s="59"/>
-      <c r="F17" s="59"/>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="57"/>
     </row>
     <row r="18" spans="1:6" s="31" customFormat="1" ht="12.75">
-      <c r="A18" s="59" t="s">
+      <c r="A18" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57"/>
     </row>
     <row r="19" spans="1:6" s="31" customFormat="1" ht="12.75">
       <c r="A19" s="34"/>
@@ -1463,7 +1457,7 @@
       <c r="C21" s="34"/>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
-      <c r="F21" s="58"/>
+      <c r="F21" s="56"/>
     </row>
     <row r="22" spans="1:6" s="31" customFormat="1" ht="29.1" customHeight="1">
       <c r="A22" s="42" t="s">
@@ -1475,15 +1469,15 @@
       <c r="C22" s="43"/>
       <c r="D22" s="44"/>
       <c r="E22" s="44"/>
-      <c r="F22" s="57"/>
+      <c r="F22" s="55"/>
     </row>
     <row r="23" spans="1:6" s="31" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A23" s="59" t="s">
+      <c r="A23" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="59"/>
+      <c r="B23" s="57"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="57"/>
       <c r="E23" s="44"/>
       <c r="F23" s="44"/>
     </row>
@@ -1500,10 +1494,10 @@
       <c r="F24" s="44"/>
     </row>
     <row r="25" spans="1:6" s="31" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A25" s="59" t="s">
+      <c r="A25" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="59"/>
+      <c r="B25" s="57"/>
       <c r="C25" s="45" t="s">
         <v>5</v>
       </c>
@@ -1515,18 +1509,18 @@
         <v>31</v>
       </c>
       <c r="B26" s="44"/>
-      <c r="C26" s="63" t="s">
+      <c r="C26" s="58" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
     </row>
     <row r="27" spans="1:6" s="31" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A27" s="59" t="s">
+      <c r="A27" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="59"/>
+      <c r="B27" s="57"/>
       <c r="C27" s="45" t="s">
         <v>34</v>
       </c>
@@ -1559,24 +1553,19 @@
       <c r="E30" s="44"/>
     </row>
     <row r="31" spans="1:6" s="31" customFormat="1" ht="116.65" customHeight="1">
-      <c r="A31" s="64" t="s">
+      <c r="A31" s="59" t="s">
         <v>38</v>
       </c>
-      <c r="B31" s="64"/>
+      <c r="B31" s="59"/>
       <c r="C31" s="48"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="64" t="s">
+      <c r="E31" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="64"/>
+      <c r="F31" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="E31:F31"/>
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A23:D23"/>
@@ -1585,6 +1574,11 @@
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="E31:F31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B16" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
@@ -1602,10 +1596,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -1626,70 +1620,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="38.25" customHeight="1">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
     </row>
     <row r="2" spans="1:7" ht="24" customHeight="1">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
     </row>
     <row r="3" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="67"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="67"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
     </row>
     <row r="6" spans="1:7" ht="39" customHeight="1">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="65" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="F7" s="23" t="s">
@@ -1809,125 +1803,114 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" s="15" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A22" s="28"/>
-      <c r="F22" s="5"/>
+    <row r="22" spans="1:7" s="15" customFormat="1" ht="42" customHeight="1">
+      <c r="A22" s="66" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="21"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" s="15" customFormat="1" ht="27.75" customHeight="1">
-      <c r="A23" s="55"/>
-      <c r="B23" s="55"/>
-      <c r="C23" s="56"/>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:7" s="15" customFormat="1" ht="42" customHeight="1">
-      <c r="A24" s="71" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" s="71"/>
-      <c r="C24" s="71"/>
-      <c r="D24" s="21"/>
+    <row r="23" spans="1:7" s="15" customFormat="1" ht="56.25" customHeight="1">
+      <c r="A23" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="67" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+    </row>
+    <row r="24" spans="1:7" s="15" customFormat="1" ht="57.4" customHeight="1">
+      <c r="A24" s="64" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="64"/>
+      <c r="C24" s="64"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" s="15" customFormat="1" ht="75.95" customHeight="1">
-      <c r="A25" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="72" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="72"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="72"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="72"/>
-    </row>
-    <row r="26" spans="1:7" s="15" customFormat="1" ht="57.4" customHeight="1">
-      <c r="A26" s="69" t="s">
-        <v>72</v>
-      </c>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="5"/>
-    </row>
-    <row r="27" spans="1:7" s="15" customFormat="1" ht="24.75" customHeight="1">
-      <c r="A27" s="68" t="s">
+    <row r="25" spans="1:7" s="15" customFormat="1" ht="24.75" customHeight="1">
+      <c r="A25" s="63" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="68"/>
-      <c r="C27" s="68"/>
-      <c r="D27" s="68"/>
-      <c r="E27" s="68"/>
-      <c r="F27" s="68"/>
-      <c r="G27" s="68"/>
-    </row>
-    <row r="28" spans="1:7" s="15" customFormat="1" ht="27" customHeight="1">
-      <c r="A28" s="68" t="s">
+      <c r="B25" s="63"/>
+      <c r="C25" s="63"/>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="63"/>
+    </row>
+    <row r="26" spans="1:7" s="15" customFormat="1" ht="27" customHeight="1">
+      <c r="A26" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="B28" s="68"/>
-      <c r="C28" s="68"/>
-      <c r="D28" s="68"/>
-      <c r="E28" s="68"/>
-      <c r="F28" s="68"/>
-      <c r="G28" s="68"/>
-    </row>
-    <row r="29" spans="1:7" s="15" customFormat="1" ht="42" customHeight="1">
-      <c r="F29" s="5" t="s">
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+    </row>
+    <row r="27" spans="1:7" s="15" customFormat="1" ht="42" customHeight="1">
+      <c r="F27" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="G27" s="5"/>
+    </row>
+    <row r="28" spans="1:7" s="15" customFormat="1" ht="24" customHeight="1">
+      <c r="F28" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" s="15" customFormat="1" ht="69.75" customHeight="1">
       <c r="G29" s="5"/>
     </row>
-    <row r="30" spans="1:7" s="15" customFormat="1" ht="24" customHeight="1">
-      <c r="F30" s="30" t="s">
-        <v>68</v>
-      </c>
+    <row r="30" spans="1:7" s="15" customFormat="1" ht="42" customHeight="1">
       <c r="G30" s="5"/>
     </row>
-    <row r="31" spans="1:7" s="15" customFormat="1" ht="69.75" customHeight="1">
-      <c r="G31" s="5"/>
-    </row>
-    <row r="32" spans="1:7" s="15" customFormat="1" ht="42" customHeight="1">
-      <c r="G32" s="5"/>
-    </row>
+    <row r="31" spans="1:7" ht="27.75" customHeight="1"/>
+    <row r="32" spans="1:7" ht="27.75" customHeight="1"/>
     <row r="33" ht="27.75" customHeight="1"/>
-    <row r="34" ht="27.75" customHeight="1"/>
-    <row r="35" ht="27.75" customHeight="1"/>
-    <row r="36" ht="24.75" customHeight="1"/>
+    <row r="34" ht="24.75" customHeight="1"/>
+    <row r="35" ht="21" customHeight="1"/>
+    <row r="36" ht="21" customHeight="1"/>
     <row r="37" ht="21" customHeight="1"/>
     <row r="38" ht="21" customHeight="1"/>
     <row r="39" ht="21" customHeight="1"/>
     <row r="40" ht="21" customHeight="1"/>
     <row r="41" ht="21" customHeight="1"/>
     <row r="42" ht="21" customHeight="1"/>
-    <row r="43" ht="21" customHeight="1"/>
+    <row r="43" ht="25.5" customHeight="1"/>
     <row r="44" ht="21" customHeight="1"/>
-    <row r="45" ht="25.5" customHeight="1"/>
+    <row r="45" ht="21" customHeight="1"/>
     <row r="46" ht="21" customHeight="1"/>
     <row r="47" ht="21" customHeight="1"/>
     <row r="48" ht="21" customHeight="1"/>
-    <row r="49" ht="21" customHeight="1"/>
-    <row r="50" ht="21" customHeight="1"/>
-    <row r="51" ht="17.25" customHeight="1"/>
-    <row r="63" ht="15" customHeight="1"/>
+    <row r="49" ht="17.25" customHeight="1"/>
+    <row r="61" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A28:G28"/>
-    <mergeCell ref="A27:G27"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="B25:G25"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A26:G26"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="B23:G23"/>
   </mergeCells>
-  <conditionalFormatting sqref="J24:J35">
+  <conditionalFormatting sqref="J22:J33">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
     <cfRule type="uniqueValues" priority="2" stopIfTrue="1"/>
   </conditionalFormatting>
@@ -1945,8 +1928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="27" customHeight="1"/>
@@ -1971,90 +1954,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="27" customHeight="1">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="27" customHeight="1">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
     </row>
     <row r="3" spans="1:11" ht="27" customHeight="1">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
-      <c r="I3" s="74"/>
+      <c r="B3" s="77"/>
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="27" customHeight="1">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="75"/>
-      <c r="D4" s="75"/>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="78"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
+      <c r="I4" s="78"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" ht="27" customHeight="1">
-      <c r="A5" s="76" t="s">
+      <c r="A5" s="79" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
-      <c r="G5" s="76"/>
-      <c r="H5" s="76"/>
-      <c r="I5" s="76"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" ht="27" customHeight="1">
-      <c r="A6" s="70" t="s">
+      <c r="A6" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="70"/>
-      <c r="C6" s="70"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="70"/>
-      <c r="I6" s="70"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
@@ -2125,14 +2108,14 @@
       <c r="I13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="27" customHeight="1">
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="79"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73"/>
       <c r="I14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="27" customHeight="1">
@@ -2190,50 +2173,50 @@
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
       <c r="I21" s="5"/>
-      <c r="L21" s="73"/>
+      <c r="L21" s="76"/>
     </row>
     <row r="22" spans="1:12" ht="27" customHeight="1">
-      <c r="A22" s="80" t="s">
+      <c r="A22" s="74" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="80"/>
-      <c r="C22" s="80"/>
+      <c r="B22" s="74"/>
+      <c r="C22" s="74"/>
       <c r="D22" s="21"/>
       <c r="E22" s="21"/>
       <c r="F22" s="20"/>
       <c r="G22" s="20"/>
       <c r="H22" s="20"/>
       <c r="I22" s="5"/>
-      <c r="L22" s="73"/>
+      <c r="L22" s="76"/>
     </row>
     <row r="23" spans="1:12" ht="42" customHeight="1">
       <c r="A23" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="81" t="s">
+      <c r="B23" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="81"/>
-      <c r="D23" s="81"/>
-      <c r="E23" s="81"/>
-      <c r="F23" s="81"/>
-      <c r="G23" s="81"/>
-      <c r="H23" s="81"/>
-      <c r="I23" s="81"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
       <c r="L23" s="12"/>
     </row>
-    <row r="24" spans="1:12" ht="49.35" customHeight="1">
-      <c r="A24" s="77" t="s">
+    <row r="24" spans="1:12" ht="42.75" customHeight="1">
+      <c r="A24" s="71" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="77"/>
-      <c r="C24" s="77"/>
-      <c r="D24" s="77"/>
-      <c r="E24" s="77"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="77"/>
-      <c r="H24" s="77"/>
-      <c r="I24" s="77"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="71"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
       <c r="L24" s="12"/>
@@ -2268,8 +2251,8 @@
       <c r="H28" s="24"/>
     </row>
     <row r="30" spans="1:12" ht="27" customHeight="1">
-      <c r="J30" s="78"/>
-      <c r="K30" s="78"/>
+      <c r="J30" s="72"/>
+      <c r="K30" s="72"/>
     </row>
     <row r="31" spans="1:12" ht="27" customHeight="1">
       <c r="H31" s="7"/>
@@ -2278,18 +2261,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:I5"/>
     <mergeCell ref="A24:I24"/>
     <mergeCell ref="J30:K30"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="B14:G14"/>
     <mergeCell ref="A22:C22"/>
     <mergeCell ref="B23:I23"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="N22:N34">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>

</xml_diff>

<commit_message>
fixing the fob replacement
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/HAPPY.xlsx
+++ b/invoice_gen/TEMPLATE/HAPPY.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\automate invoice\invoice_gen\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E34C8C-8771-4515-B5E2-4BAC69FF3155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D871B829-4A07-435B-838A-64FAB50BF654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
   <si>
     <t>SALES CONTRACT</t>
   </si>
@@ -129,12 +129,6 @@
   </si>
   <si>
     <t>Người bán, người mua và người thụ hưởng đã thống nhất đồng ý các giao dịch sau theo các điều khoản và điều kiện được quy định dưới đây:</t>
-  </si>
-  <si>
-    <t>FCA:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BAVET,SVAYRIENG </t>
   </si>
   <si>
     <t>Term of Payment: 100% TT after shipment
@@ -346,6 +340,9 @@
   </si>
   <si>
     <t>JFINV</t>
+  </si>
+  <si>
+    <t>FCA: BAVET,SVAYRIENG</t>
   </si>
 </sst>
 </file>
@@ -711,9 +708,6 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="4" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -773,6 +767,9 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="16" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1226,41 +1223,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="49" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="49" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" style="49" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="49" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" style="49" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" style="49" customWidth="1"/>
-    <col min="7" max="16382" width="28.7109375" style="49" customWidth="1"/>
-    <col min="16383" max="16384" width="28.7109375" style="49"/>
+    <col min="1" max="1" width="24.42578125" style="48" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" style="48" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" style="48" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="48" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" style="48" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" style="48" customWidth="1"/>
+    <col min="7" max="16382" width="28.7109375" style="48" customWidth="1"/>
+    <col min="16383" max="16384" width="28.7109375" style="48"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="31" customFormat="1" ht="45.95" customHeight="1">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
     </row>
     <row r="2" spans="1:6" s="20" customFormat="1" ht="27" customHeight="1">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
+      <c r="F2" s="59"/>
     </row>
     <row r="3" spans="1:6" s="31" customFormat="1" ht="27" customHeight="1">
       <c r="B3" s="32"/>
@@ -1268,8 +1265,8 @@
       <c r="E3" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="53" t="s">
-        <v>76</v>
+      <c r="F3" s="52" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="31" customFormat="1" ht="30" customHeight="1">
@@ -1279,21 +1276,21 @@
       <c r="E4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="54" t="s">
-        <v>78</v>
+      <c r="F4" s="53" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="31" customFormat="1" ht="25.5">
       <c r="A5" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="61"/>
-      <c r="F5" s="61"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="60"/>
     </row>
     <row r="6" spans="1:6" s="31" customFormat="1" ht="27.75" customHeight="1">
       <c r="A6" s="33" t="s">
@@ -1348,25 +1345,25 @@
       <c r="A11" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
+      <c r="C11" s="60"/>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="60"/>
     </row>
     <row r="12" spans="1:6" s="37" customFormat="1" ht="25.5">
       <c r="A12" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="57"/>
+      <c r="F12" s="57"/>
     </row>
     <row r="13" spans="1:6" s="37" customFormat="1" ht="30" customHeight="1">
       <c r="A13" s="34" t="s">
@@ -1417,24 +1414,24 @@
       <c r="F16" s="33"/>
     </row>
     <row r="17" spans="1:6" s="31" customFormat="1" ht="18.95" customHeight="1">
-      <c r="A17" s="57" t="s">
-        <v>74</v>
-      </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
+      <c r="A17" s="56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" s="56"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
     </row>
     <row r="18" spans="1:6" s="31" customFormat="1" ht="12.75">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
     </row>
     <row r="19" spans="1:6" s="31" customFormat="1" ht="12.75">
       <c r="A19" s="34"/>
@@ -1457,115 +1454,113 @@
       <c r="C21" s="34"/>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
-      <c r="F21" s="56"/>
-    </row>
-    <row r="22" spans="1:6" s="31" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A22" s="42" t="s">
+      <c r="F21" s="55"/>
+    </row>
+    <row r="22" spans="1:6" s="31" customFormat="1" ht="21" customHeight="1">
+      <c r="A22" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="62"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="54"/>
+    </row>
+    <row r="23" spans="1:6" s="31" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A23" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="43" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="55"/>
-    </row>
-    <row r="23" spans="1:6" s="31" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A23" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="56"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
     </row>
     <row r="24" spans="1:6" s="31" customFormat="1" ht="29.1" customHeight="1">
       <c r="A24" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+    </row>
+    <row r="25" spans="1:6" s="31" customFormat="1" ht="29.1" customHeight="1">
+      <c r="A25" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="45" t="s">
+      <c r="B25" s="56"/>
+      <c r="C25" s="44" t="s">
+        <v>5</v>
+      </c>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+    </row>
+    <row r="26" spans="1:6" s="31" customFormat="1" ht="25.5">
+      <c r="A26" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-    </row>
-    <row r="25" spans="1:6" s="31" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A25" s="57" t="s">
+      <c r="B26" s="43"/>
+      <c r="C26" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="45" t="s">
-        <v>5</v>
-      </c>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-    </row>
-    <row r="26" spans="1:6" s="31" customFormat="1" ht="51">
-      <c r="A26" s="36" t="s">
+      <c r="D26" s="57"/>
+      <c r="E26" s="57"/>
+      <c r="F26" s="57"/>
+    </row>
+    <row r="27" spans="1:6" s="31" customFormat="1" ht="28.5" customHeight="1">
+      <c r="A27" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B26" s="44"/>
-      <c r="C26" s="58" t="s">
+      <c r="B27" s="56"/>
+      <c r="C27" s="44" t="s">
         <v>32</v>
-      </c>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-    </row>
-    <row r="27" spans="1:6" s="31" customFormat="1" ht="28.5" customHeight="1">
-      <c r="A27" s="57" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="57"/>
-      <c r="C27" s="45" t="s">
-        <v>34</v>
       </c>
       <c r="D27" s="34"/>
       <c r="E27" s="34"/>
     </row>
     <row r="28" spans="1:6" s="31" customFormat="1" ht="29.1" customHeight="1">
       <c r="A28" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B28" s="43"/>
+      <c r="C28" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
+    </row>
+    <row r="29" spans="1:6" s="31" customFormat="1" ht="29.1" customHeight="1">
+      <c r="A29" s="44" t="s">
+        <v>73</v>
+      </c>
+      <c r="B29" s="43"/>
+      <c r="C29" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="44"/>
-      <c r="C28" s="46" t="s">
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+    </row>
+    <row r="30" spans="1:6" s="31" customFormat="1" ht="29.1" customHeight="1">
+      <c r="E30" s="43"/>
+    </row>
+    <row r="31" spans="1:6" s="31" customFormat="1" ht="116.65" customHeight="1">
+      <c r="A31" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="D28" s="47"/>
-      <c r="E28" s="47"/>
-    </row>
-    <row r="29" spans="1:6" s="31" customFormat="1" ht="29.1" customHeight="1">
-      <c r="A29" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-    </row>
-    <row r="30" spans="1:6" s="31" customFormat="1" ht="29.1" customHeight="1">
-      <c r="E30" s="44"/>
-    </row>
-    <row r="31" spans="1:6" s="31" customFormat="1" ht="116.65" customHeight="1">
-      <c r="A31" s="59" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="59"/>
-      <c r="C31" s="48"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="47"/>
       <c r="D31" s="34"/>
-      <c r="E31" s="59" t="s">
+      <c r="E31" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="F31" s="59"/>
+      <c r="F31" s="58"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="14">
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A18:F18"/>
     <mergeCell ref="A23:D23"/>
@@ -1574,6 +1569,7 @@
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B11:F11"/>
     <mergeCell ref="B12:F12"/>
+    <mergeCell ref="A22:B22"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="C26:F26"/>
     <mergeCell ref="A27:B27"/>
@@ -1598,8 +1594,8 @@
   </sheetPr>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -1621,7 +1617,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="38.25" customHeight="1">
       <c r="A1" s="68" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="68"/>
       <c r="C1" s="68"/>
@@ -1654,7 +1650,7 @@
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1">
       <c r="A4" s="69" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="69"/>
       <c r="C4" s="69"/>
@@ -1665,7 +1661,7 @@
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
       <c r="A5" s="70" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="70"/>
       <c r="C5" s="70"/>
@@ -1676,7 +1672,7 @@
     </row>
     <row r="6" spans="1:7" ht="39" customHeight="1">
       <c r="A6" s="65" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B6" s="65"/>
       <c r="C6" s="65"/>
@@ -1687,58 +1683,58 @@
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="F7" s="23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="15" customFormat="1" ht="30" customHeight="1">
       <c r="A8" s="25" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E8" s="26"/>
       <c r="F8" s="26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="15" customFormat="1" ht="21" customHeight="1">
       <c r="B9" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F9" s="26" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="15" customFormat="1" ht="22.5" customHeight="1">
       <c r="B10" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="15" customFormat="1" ht="20.25" customHeight="1">
       <c r="B11" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="15" customFormat="1" ht="15.75" customHeight="1">
@@ -1746,39 +1742,39 @@
     </row>
     <row r="13" spans="1:7" s="15" customFormat="1" ht="25.5" customHeight="1">
       <c r="A13" s="25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G13" s="5"/>
     </row>
     <row r="14" spans="1:7" s="15" customFormat="1" ht="25.5" customHeight="1">
       <c r="B14" s="27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
     <row r="15" spans="1:7" s="15" customFormat="1" ht="25.5" customHeight="1">
       <c r="B15" s="15" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G15" s="5"/>
     </row>
     <row r="16" spans="1:7" s="15" customFormat="1" ht="25.5" customHeight="1">
       <c r="B16" s="15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
     <row r="17" spans="1:7" s="15" customFormat="1" ht="27.75" customHeight="1">
       <c r="A17" s="28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
@@ -1805,7 +1801,7 @@
     </row>
     <row r="22" spans="1:7" s="15" customFormat="1" ht="42" customHeight="1">
       <c r="A22" s="66" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B22" s="66"/>
       <c r="C22" s="66"/>
@@ -1814,10 +1810,10 @@
     </row>
     <row r="23" spans="1:7" s="15" customFormat="1" ht="56.25" customHeight="1">
       <c r="A23" s="26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B23" s="67" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23" s="67"/>
       <c r="D23" s="67"/>
@@ -1827,7 +1823,7 @@
     </row>
     <row r="24" spans="1:7" s="15" customFormat="1" ht="57.4" customHeight="1">
       <c r="A24" s="64" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B24" s="64"/>
       <c r="C24" s="64"/>
@@ -1838,7 +1834,7 @@
     </row>
     <row r="25" spans="1:7" s="15" customFormat="1" ht="24.75" customHeight="1">
       <c r="A25" s="63" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B25" s="63"/>
       <c r="C25" s="63"/>
@@ -1849,7 +1845,7 @@
     </row>
     <row r="26" spans="1:7" s="15" customFormat="1" ht="27" customHeight="1">
       <c r="A26" s="63" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B26" s="63"/>
       <c r="C26" s="63"/>
@@ -1860,13 +1856,13 @@
     </row>
     <row r="27" spans="1:7" s="15" customFormat="1" ht="42" customHeight="1">
       <c r="F27" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" s="15" customFormat="1" ht="24" customHeight="1">
       <c r="F28" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G28" s="5"/>
     </row>
@@ -1955,7 +1951,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="27" customHeight="1">
       <c r="A1" s="68" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="68"/>
       <c r="C1" s="68"/>
@@ -1970,7 +1966,7 @@
     </row>
     <row r="2" spans="1:11" ht="27" customHeight="1">
       <c r="A2" s="69" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="69"/>
       <c r="C2" s="69"/>
@@ -1998,7 +1994,7 @@
     </row>
     <row r="4" spans="1:11" ht="27" customHeight="1">
       <c r="A4" s="78" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="78"/>
       <c r="C4" s="78"/>
@@ -2013,7 +2009,7 @@
     </row>
     <row r="5" spans="1:11" ht="27" customHeight="1">
       <c r="A5" s="79" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B5" s="79"/>
       <c r="C5" s="79"/>
@@ -2028,7 +2024,7 @@
     </row>
     <row r="6" spans="1:11" ht="27" customHeight="1">
       <c r="A6" s="65" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B6" s="65"/>
       <c r="C6" s="65"/>
@@ -2042,63 +2038,63 @@
       <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="27" customHeight="1">
-      <c r="H7" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="51" t="s">
-        <v>77</v>
+      <c r="H7" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="50" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="27" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F8" s="10"/>
       <c r="H8" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="I8" s="52" t="s">
-        <v>78</v>
+        <v>44</v>
+      </c>
+      <c r="I8" s="51" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="27" customHeight="1">
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="27" customHeight="1">
       <c r="B10" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="H10" s="12" t="str">
         <f>'[1]Invoice OJY24001'!F10</f>
         <v>Delivery term:</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:11" ht="27" customHeight="1">
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="27" customHeight="1">
       <c r="A13" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
@@ -2109,7 +2105,7 @@
     </row>
     <row r="14" spans="1:11" ht="27" customHeight="1">
       <c r="B14" s="73" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C14" s="73"/>
       <c r="D14" s="73"/>
@@ -2120,7 +2116,7 @@
     </row>
     <row r="15" spans="1:11" ht="27" customHeight="1">
       <c r="B15" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
@@ -2131,7 +2127,7 @@
     </row>
     <row r="16" spans="1:11" ht="27" customHeight="1">
       <c r="B16" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="16"/>
@@ -2142,10 +2138,10 @@
     </row>
     <row r="17" spans="1:12" ht="27" customHeight="1">
       <c r="A17" s="17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -2177,7 +2173,7 @@
     </row>
     <row r="22" spans="1:12" ht="27" customHeight="1">
       <c r="A22" s="74" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B22" s="74"/>
       <c r="C22" s="74"/>
@@ -2191,10 +2187,10 @@
     </row>
     <row r="23" spans="1:12" ht="42" customHeight="1">
       <c r="A23" s="22" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B23" s="75" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C23" s="75"/>
       <c r="D23" s="75"/>
@@ -2207,7 +2203,7 @@
     </row>
     <row r="24" spans="1:12" ht="42.75" customHeight="1">
       <c r="A24" s="71" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B24" s="71"/>
       <c r="C24" s="71"/>
@@ -2223,7 +2219,7 @@
     </row>
     <row r="25" spans="1:12" ht="27" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2238,10 +2234,10 @@
     </row>
     <row r="26" spans="1:12" s="4" customFormat="1" ht="27" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F26" s="23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="27" customHeight="1">

</xml_diff>

<commit_message>
fixing the damn desc doesnt pop in fob mode
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/HAPPY.xlsx
+++ b/invoice_gen/TEMPLATE/HAPPY.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\automate invoice\invoice_gen\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D871B829-4A07-435B-838A-64FAB50BF654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F70D3E3-AAAE-4F45-AE22-A0CC07C626B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="10" r:id="rId1"/>
     <sheet name="Invoice" sheetId="12" r:id="rId2"/>
     <sheet name="Packing list" sheetId="9" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$1:$F$34</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$G$29</definedName>
@@ -43,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="78">
   <si>
     <t>SALES CONTRACT</t>
   </si>
@@ -838,129 +835,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>203200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>179236</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>347731</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="2" name="Group 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="10679029" y="10008937"/>
-          <a:ext cx="3025707" cy="1327636"/>
-          <a:chOff x="7095490" y="13465334"/>
-          <a:chExt cx="4610436" cy="2150203"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="3" name="图片 1" descr="微信图片_20231124163951">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="7095490" y="13465334"/>
-            <a:ext cx="2990673" cy="1817845"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-      </xdr:pic>
-      <xdr:pic>
-        <xdr:nvPicPr>
-          <xdr:cNvPr id="4" name="图片 2" descr="微信图片_20231124163945">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
-          </xdr:cNvPicPr>
-        </xdr:nvPicPr>
-        <xdr:blipFill>
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-          <a:stretch>
-            <a:fillRect/>
-          </a:stretch>
-        </xdr:blipFill>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="9526289" y="14283149"/>
-            <a:ext cx="2179637" cy="1332388"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-        </xdr:spPr>
-      </xdr:pic>
-    </xdr:grpSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Contract"/>
-      <sheetName val="Packing list"/>
-      <sheetName val="Invoice OJY24001"/>
-      <sheetName val="Invoice OJY24001 SIGN"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="10">
-          <cell r="F10" t="str">
-            <v>Delivery term:</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1223,14 +1097,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:B22"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.42578125" style="48" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" style="48" customWidth="1"/>
+    <col min="2" max="2" width="35.28515625" style="48" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" style="48" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" style="48" customWidth="1"/>
     <col min="5" max="5" width="17.140625" style="48" customWidth="1"/>
@@ -1594,8 +1468,8 @@
   </sheetPr>
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -1916,7 +1790,6 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="7" max="1048575" man="1"/>
   </colBreaks>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1924,8 +1797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A50" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="27" customHeight="1"/>
@@ -2075,9 +1948,8 @@
       <c r="B10" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="12" t="str">
-        <f>'[1]Invoice OJY24001'!F10</f>
-        <v>Delivery term:</v>
+      <c r="H10" s="12" t="s">
+        <v>61</v>
       </c>
       <c r="I10" s="12" t="s">
         <v>48</v>

</xml_diff>